<commit_message>
Updated the true clone pairs and recovered the CheckEqualsMethodsAndGettersSetters.java to work with SO+Qualitas again
</commit_message>
<xml_diff>
--- a/PLATINUM_FINAL_ok+good_130901_A+B+C.xlsx
+++ b/PLATINUM_FINAL_ok+good_130901_A+B+C.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27713"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27715"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27000" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="GOLD_ok+good_130901_A+B+C" sheetId="1" r:id="rId1"/>
@@ -6708,7 +6708,7 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -6770,6 +6770,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
@@ -7314,8 +7315,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB493"/>
   <sheetViews>
-    <sheetView topLeftCell="X73" workbookViewId="0">
-      <selection activeCell="Z74" sqref="Z74"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="V74" sqref="V74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7324,7 +7325,7 @@
     <col min="2" max="2" width="3.5" style="1" customWidth="1"/>
     <col min="3" max="3" width="36.5" style="1" customWidth="1"/>
     <col min="4" max="5" width="4.1640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="179.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="88.83203125" style="1" customWidth="1"/>
     <col min="7" max="9" width="10.6640625" style="1" customWidth="1"/>
     <col min="10" max="14" width="2.6640625" style="1" customWidth="1"/>
     <col min="15" max="15" width="18" style="1" bestFit="1" customWidth="1"/>
@@ -8782,7 +8783,7 @@
       <c r="AA25"/>
       <c r="AB25"/>
     </row>
-    <row r="26" spans="1:28" ht="409" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>0</v>
       </c>
@@ -8818,10 +8819,10 @@
       <c r="U26" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="V26" s="6" t="s">
+      <c r="V26" s="1" t="s">
         <v>815</v>
       </c>
-      <c r="W26" s="6" t="s">
+      <c r="W26" s="1" t="s">
         <v>816</v>
       </c>
       <c r="X26" s="26">
@@ -8830,7 +8831,7 @@
       <c r="Y26" s="26">
         <v>41415</v>
       </c>
-      <c r="Z26" s="6" t="s">
+      <c r="Z26" s="1" t="s">
         <v>817</v>
       </c>
       <c r="AA26"/>
@@ -11430,7 +11431,7 @@
         <v>41430</v>
       </c>
     </row>
-    <row r="72" spans="1:28" customFormat="1" ht="409" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>0</v>
       </c>
@@ -11467,23 +11468,23 @@
       <c r="U72" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="V72" s="6" t="s">
+      <c r="V72" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="W72" s="6" t="s">
+      <c r="W72" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="X72" s="26">
+      <c r="X72" s="27">
         <v>40263</v>
       </c>
-      <c r="Y72" s="26">
+      <c r="Y72" s="27">
         <v>41430</v>
       </c>
-      <c r="Z72" s="6" t="s">
+      <c r="Z72" s="1" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="73" spans="1:28" customFormat="1" ht="409" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -11520,23 +11521,23 @@
       <c r="U73" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="V73" s="6" t="s">
+      <c r="V73" s="1" t="s">
         <v>809</v>
       </c>
-      <c r="W73" s="6" t="s">
+      <c r="W73" s="1" t="s">
         <v>810</v>
       </c>
-      <c r="X73" s="26">
+      <c r="X73" s="27">
         <v>40264</v>
       </c>
-      <c r="Y73" s="26">
+      <c r="Y73" s="27">
         <v>41430</v>
       </c>
-      <c r="Z73" s="6" t="s">
+      <c r="Z73" s="1" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="74" spans="1:28" customFormat="1" ht="240" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:28" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
         <v>0</v>
       </c>
@@ -11573,19 +11574,19 @@
       <c r="U74" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="V74" s="6" t="s">
+      <c r="V74" s="1" t="s">
         <v>814</v>
       </c>
-      <c r="W74" s="6" t="s">
+      <c r="W74" s="1" t="s">
         <v>813</v>
       </c>
-      <c r="X74" s="26">
+      <c r="X74" s="27">
         <v>40265</v>
       </c>
-      <c r="Y74" s="26">
+      <c r="Y74" s="27">
         <v>41430</v>
       </c>
-      <c r="Z74" s="6" t="s">
+      <c r="Z74" s="1" t="s">
         <v>812</v>
       </c>
     </row>
@@ -30528,7 +30529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>

</xml_diff>